<commit_message>
April 2025 update without ECB
</commit_message>
<xml_diff>
--- a/MSC_mean.xlsx
+++ b/MSC_mean.xlsx
@@ -69,7 +69,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C561"/>
+  <dimension ref="A1:C567"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6246,6 +6246,72 @@
         <v>3</v>
       </c>
     </row>
+    <row r="562">
+      <c r="A562" s="1">
+        <v>45536</v>
+      </c>
+      <c r="B562" s="2">
+        <v>3.0439546237485131</v>
+      </c>
+      <c r="C562" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="1">
+        <v>45566</v>
+      </c>
+      <c r="B563" s="2">
+        <v>2.8981559020643028</v>
+      </c>
+      <c r="C563" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="1">
+        <v>45597</v>
+      </c>
+      <c r="B564" s="2">
+        <v>2.0403693875787057</v>
+      </c>
+      <c r="C564" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B565" s="2">
+        <v>2.288815139456557</v>
+      </c>
+      <c r="C565" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B566" s="2">
+        <v>3.6692668713944512</v>
+      </c>
+      <c r="C566" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="1">
+        <v>45689</v>
+      </c>
+      <c r="B567" s="2">
+        <v>4.0335035493262668</v>
+      </c>
+      <c r="C567" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>